<commit_message>
[ADD] Sign up, Login, Android Project
</commit_message>
<xml_diff>
--- a/CommutincationInfo.xlsx
+++ b/CommutincationInfo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seosanghyeon/Matcher/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seosanghyeon/git/Matcher/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8054E98A-B596-DD4C-A977-41BE53C18BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCC87BB-5DA3-474D-BD5B-4D6920B764CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36000" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{5B7FD093-8346-A54D-A2F7-F6B1F89C7B17}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21060" xr2:uid="{5B7FD093-8346-A54D-A2F7-F6B1F89C7B17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>URL Pattern</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -111,6 +111,21 @@
   </si>
   <si>
     <t>chatId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoginDTO(id, password)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MemberDTO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NoSuchElementException</t>
+  </si>
+  <si>
+    <t>HttpServletResponse_OK</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -475,18 +490,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3375E223-1BE2-4948-AB5B-923035C53DA7}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -516,16 +531,25 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
       <c r="I2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
       </c>
       <c r="I4" t="s">
         <v>9</v>
@@ -557,6 +581,11 @@
       </c>
       <c r="H8" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="H11" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[ADD] Friend Fragment ListView
</commit_message>
<xml_diff>
--- a/CommutincationInfo.xlsx
+++ b/CommutincationInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seosanghyeon/git/Matcher/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCC87BB-5DA3-474D-BD5B-4D6920B764CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48B7A5A-DB52-3D49-B234-23A53DED7391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21060" xr2:uid="{5B7FD093-8346-A54D-A2F7-F6B1F89C7B17}"/>
+    <workbookView xWindow="20" yWindow="880" windowWidth="36000" windowHeight="21060" xr2:uid="{5B7FD093-8346-A54D-A2F7-F6B1F89C7B17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>URL Pattern</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -46,10 +46,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/profile</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/{userId}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -122,10 +118,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>NoSuchElementException</t>
-  </si>
-  <si>
     <t>HttpServletResponse_OK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/member</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/signup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -490,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3375E223-1BE2-4948-AB5B-923035C53DA7}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -501,91 +506,98 @@
     <col min="1" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
         <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
         <v>8</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
       <c r="I6" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
         <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="H11" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>